<commit_message>
updated growth to growth management
</commit_message>
<xml_diff>
--- a/data/activity-challenge.xlsx
+++ b/data/activity-challenge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://psrcwa-my.sharepoint.com/personal/chelmann_psrc_org/Documents/coding/psrc-activity-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{A7D2FF3F-C1BA-493C-915D-5D9EDF01FC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F047D57A-96E9-48C5-AAB0-B1D2A899F624}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{A7D2FF3F-C1BA-493C-915D-5D9EDF01FC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52479AEC-F91E-4C4B-9CFD-66D7324913CE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C374EE61-D86A-4A0C-A22D-10A072C9E93B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{C374EE61-D86A-4A0C-A22D-10A072C9E93B}"/>
   </bookViews>
   <sheets>
     <sheet name="miles" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
     <t>mountain</t>
   </si>
   <si>
-    <t>Growth</t>
+    <t>Growth Management</t>
   </si>
 </sst>
 </file>
@@ -1307,19 +1307,19 @@
   <dimension ref="A1:BC70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="55" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="55" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>34.4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>107</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>108</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>116</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>118</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>120</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>123</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>126</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>127</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>128</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>129</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>131</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>133</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
updated person miles to round to 1 decimal
</commit_message>
<xml_diff>
--- a/data/activity-challenge.xlsx
+++ b/data/activity-challenge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://psrcwa-my.sharepoint.com/personal/chelmann_psrc_org/Documents/coding/psrc-activity-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{A7D2FF3F-C1BA-493C-915D-5D9EDF01FC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52479AEC-F91E-4C4B-9CFD-66D7324913CE}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{A7D2FF3F-C1BA-493C-915D-5D9EDF01FC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52F3EE34-0708-46B9-8E88-E837A42A8D99}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{C374EE61-D86A-4A0C-A22D-10A072C9E93B}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C374EE61-D86A-4A0C-A22D-10A072C9E93B}"/>
   </bookViews>
   <sheets>
     <sheet name="miles" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="138">
   <si>
     <t>Name</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>mountain</t>
+  </si>
+  <si>
+    <t>rebel</t>
   </si>
   <si>
     <t>Growth Management</t>
@@ -450,7 +453,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,6 +584,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -927,8 +937,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1306,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE3DDF3-FFF1-4DBE-8834-A3E5309DE089}">
   <dimension ref="A1:BC70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1487,1111 +1499,1695 @@
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>17.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>19.8</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>24.2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>28.4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>25.9</v>
       </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>12.1</v>
       </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>11.5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>10.8</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>13</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>9</v>
       </c>
+      <c r="H13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="D15" s="1">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1">
+        <v>33.6</v>
+      </c>
+      <c r="F15" s="1">
+        <v>28.7</v>
+      </c>
+      <c r="G15" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>22.3</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>40.5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>39.200000000000003</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>23.9</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>19.7</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>22.9</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>24.1</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>24.2</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>23.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="J21" s="2"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>2.6</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>11.3</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>10.4</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="H25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>18.399999999999999</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>23.7</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>31</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>27.2</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>8.6</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>20.5</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>21.2</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>26.3</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>20.100000000000001</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>35.799999999999997</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>44.6</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>45.9</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1">
         <v>37.299999999999997</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>19.100000000000001</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>27.3</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>40.799999999999997</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>38</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1">
         <v>29.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>12.7</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>18.7</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>13.9</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>36.4</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>35.4</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
         <v>33.700000000000003</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="1">
         <v>32.200000000000003</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>17.2</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>16.3</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>23.9</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
         <v>38.5</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="1">
         <v>34.4</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>17.899999999999999</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>30.6</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>32.6</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="1">
         <v>41.1</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="1">
         <v>30.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>11.9</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>15.1</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>14.6</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
         <v>16.899999999999999</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="1">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>5.4</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>15.6</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>24.3</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <v>26</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="1">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="1">
+        <v>13</v>
+      </c>
+      <c r="E45" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="G45" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E47" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="1">
+        <v>20.9</v>
+      </c>
+      <c r="E48" s="1">
+        <v>23</v>
+      </c>
+      <c r="F48" s="1">
+        <v>23.6</v>
+      </c>
+      <c r="G48" s="1">
+        <v>29.3</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>31.1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="G50" s="1">
+        <v>34.9</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45">
-        <v>13</v>
-      </c>
-      <c r="E45">
-        <v>25.1</v>
-      </c>
-      <c r="F45">
-        <v>20.5</v>
-      </c>
-      <c r="G45">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47">
+      <c r="D51" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="E51" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="F51" s="1">
+        <v>23.3</v>
+      </c>
+      <c r="G51" s="1">
+        <v>31</v>
+      </c>
+      <c r="H51" s="1">
+        <v>31.2</v>
+      </c>
+      <c r="J51" s="2"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E53" s="1">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="F53" s="1">
+        <v>32.4</v>
+      </c>
+      <c r="G53" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="H53" s="1">
+        <v>35.9</v>
+      </c>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="1">
         <v>5.4</v>
       </c>
-      <c r="E47">
-        <v>18.899999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>108</v>
-      </c>
-      <c r="B48" t="s">
-        <v>136</v>
-      </c>
-      <c r="C48" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48">
-        <v>20.9</v>
-      </c>
-      <c r="E48">
-        <v>23</v>
-      </c>
-      <c r="F48">
-        <v>23.6</v>
-      </c>
-      <c r="G48">
-        <v>29.3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B49" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50">
-        <v>16.2</v>
-      </c>
-      <c r="E50">
-        <v>31.1</v>
-      </c>
-      <c r="F50">
-        <v>32.9</v>
-      </c>
-      <c r="G50">
-        <v>34.9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="E54" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="F54" s="1">
+        <v>21.1</v>
+      </c>
+      <c r="G54" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="H54" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C55" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D51">
-        <v>10.4</v>
-      </c>
-      <c r="E51">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="F51">
-        <v>23.3</v>
-      </c>
-      <c r="G51">
-        <v>31</v>
-      </c>
-      <c r="H51">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C56" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>115</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="D56" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="E56" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="F56" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="G56" s="1">
+        <v>35.9</v>
+      </c>
+      <c r="H56" s="1">
+        <v>41</v>
+      </c>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D53">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="E53">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="F53">
-        <v>32.4</v>
-      </c>
-      <c r="G53">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="H53">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D62" s="1">
+        <v>20</v>
+      </c>
+      <c r="E62" s="1">
         <v>35.9</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>116</v>
-      </c>
-      <c r="B54" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" t="s">
-        <v>113</v>
-      </c>
-      <c r="D54">
-        <v>5.4</v>
-      </c>
-      <c r="E54">
-        <v>12.9</v>
-      </c>
-      <c r="F54">
-        <v>21.1</v>
-      </c>
-      <c r="G54">
-        <v>15.2</v>
-      </c>
-      <c r="H54">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>117</v>
-      </c>
-      <c r="B55" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56">
-        <v>27.4</v>
-      </c>
-      <c r="E56">
-        <v>37.6</v>
-      </c>
-      <c r="F56">
-        <v>37.6</v>
-      </c>
-      <c r="G56">
-        <v>35.9</v>
-      </c>
-      <c r="H56">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>119</v>
-      </c>
-      <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="F62" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="G62" s="1">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="H62" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C63" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>123</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C64" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>124</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C65" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>125</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C66" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>126</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C67" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D62">
-        <v>20</v>
-      </c>
-      <c r="E62">
-        <v>35.9</v>
-      </c>
-      <c r="F62">
-        <v>36.9</v>
-      </c>
-      <c r="G62">
-        <v>40.700000000000003</v>
-      </c>
-      <c r="H62">
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D70" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="E70" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="F70" s="1">
+        <v>31.9</v>
+      </c>
+      <c r="G70" s="1">
         <v>37.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>127</v>
-      </c>
-      <c r="B63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" t="s">
-        <v>121</v>
-      </c>
-      <c r="C64" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>129</v>
-      </c>
-      <c r="B65" t="s">
-        <v>121</v>
-      </c>
-      <c r="C65" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>130</v>
-      </c>
-      <c r="B66" t="s">
-        <v>121</v>
-      </c>
-      <c r="C66" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>131</v>
-      </c>
-      <c r="B67" t="s">
-        <v>121</v>
-      </c>
-      <c r="C67" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>132</v>
-      </c>
-      <c r="B68" t="s">
-        <v>121</v>
-      </c>
-      <c r="C68" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>133</v>
-      </c>
-      <c r="B69" t="s">
-        <v>121</v>
-      </c>
-      <c r="C69" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>134</v>
-      </c>
-      <c r="B70" t="s">
-        <v>121</v>
-      </c>
-      <c r="C70" t="s">
-        <v>122</v>
-      </c>
-      <c r="D70">
-        <v>12.5</v>
-      </c>
-      <c r="E70">
-        <v>20.8</v>
-      </c>
-      <c r="F70">
-        <v>31.9</v>
-      </c>
-      <c r="G70">
-        <v>37.5</v>
-      </c>
-      <c r="H70">
+      <c r="H70" s="1">
         <v>23.5</v>
       </c>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>